<commit_message>
Correção do artefato 17
</commit_message>
<xml_diff>
--- a/17. Análise de eventos.xlsx
+++ b/17. Análise de eventos.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="36">
   <si>
     <t>Externo</t>
   </si>
@@ -46,19 +46,16 @@
     <t>Extemporâneo</t>
   </si>
   <si>
-    <t>Solicitar disponibilidade de produtos</t>
+    <t>Vender produtos da loja</t>
   </si>
   <si>
     <t>FB</t>
   </si>
   <si>
-    <t>Cliente solicita disponibilidade de produtos</t>
+    <t>Loja fornece informações sobre produtos para venda</t>
   </si>
   <si>
     <t>x</t>
-  </si>
-  <si>
-    <t>Realizar pedido de compra</t>
   </si>
   <si>
     <t>Cliente realiza o pedido de compra</t>
@@ -67,53 +64,68 @@
     <t>x(1)</t>
   </si>
   <si>
-    <t>Realizar pagamento</t>
+    <t>Pagar compra de produtos</t>
+  </si>
+  <si>
+    <t>Cliente solicita orçamento do pedido de compra</t>
+  </si>
+  <si>
+    <t>x(2)</t>
+  </si>
+  <si>
+    <t>Loja encaminha orçamento</t>
+  </si>
+  <si>
+    <t>x(3)</t>
   </si>
   <si>
     <t>Cliente realiza pagamento do pedido</t>
   </si>
   <si>
-    <t>x(2)</t>
+    <t>x(4)</t>
+  </si>
+  <si>
+    <t>Cancelar compra</t>
   </si>
   <si>
     <t>FA</t>
   </si>
   <si>
-    <t>Loja não recebe o pagamento</t>
-  </si>
-  <si>
-    <t>x(3)</t>
-  </si>
-  <si>
-    <t>Cliente informa o motivo do não pagamento</t>
-  </si>
-  <si>
-    <t>x(4)</t>
-  </si>
-  <si>
-    <t>Solicitar prazo de entrega</t>
-  </si>
-  <si>
-    <t>Loja informa prazo de entrega do produto</t>
+    <t>Loja não recebe o pagamento do pedido</t>
   </si>
   <si>
     <t>x(5)</t>
   </si>
   <si>
-    <t>Entregar pedido de compra</t>
+    <t>Cliente informa motivo do não pagamento</t>
   </si>
   <si>
-    <t>Correio realiza entrega do pedido</t>
+    <t>x(6,7)</t>
   </si>
   <si>
-    <t>x(6)</t>
+    <t>Devolver produto</t>
+  </si>
+  <si>
+    <t>Cliente realiza devolutiva dos produtos</t>
+  </si>
+  <si>
+    <t>x(8)</t>
+  </si>
+  <si>
+    <t>Receber produto</t>
+  </si>
+  <si>
+    <t>Entregador realiza entrega do pedido de compra</t>
+  </si>
+  <si>
+    <t>x(9)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -135,6 +147,10 @@
       <b/>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10.0"/>
       <name val="Arial"/>
     </font>
     <font>
@@ -186,8 +202,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00FFFF"/>
-        <bgColor rgb="FF00FFFF"/>
+        <fgColor rgb="FFFF9900"/>
+        <bgColor rgb="FFFF9900"/>
       </patternFill>
     </fill>
     <fill>
@@ -198,8 +214,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF9900"/>
-        <bgColor rgb="FFFF9900"/>
+        <fgColor rgb="FF00FFFF"/>
+        <bgColor rgb="FF00FFFF"/>
       </patternFill>
     </fill>
     <fill>
@@ -310,9 +326,6 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
     </border>
     <border>
       <left style="thin">
@@ -321,6 +334,9 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
     </border>
   </borders>
   <cellStyleXfs count="1">
@@ -356,16 +372,16 @@
     <xf borderId="11" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" textRotation="90" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="7" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" textRotation="90" vertical="center"/>
+    <xf borderId="7" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" textRotation="90" vertical="center"/>
     </xf>
     <xf borderId="10" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="10" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    <xf borderId="10" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="10" fillId="4" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="10" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="10" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
@@ -374,39 +390,39 @@
     <xf borderId="10" fillId="6" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf borderId="12" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="11" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="10" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
     <xf borderId="11" fillId="7" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" textRotation="90" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="12" fillId="8" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" textRotation="90" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="10" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="10" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="10" fillId="5" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="10" fillId="5" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="12" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="7" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="10" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="7" fillId="8" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" textRotation="90" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="12" fillId="9" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" textRotation="90" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="10" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" textRotation="90" vertical="center"/>
     </xf>
-    <xf borderId="11" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="11" fillId="9" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="10" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="12" fillId="10" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" textRotation="90" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="11" fillId="10" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" textRotation="90" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="10" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" textRotation="90" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -697,40 +713,36 @@
       <c r="D3" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16" t="s">
+      <c r="E3" s="16" t="s">
         <v>14</v>
       </c>
+      <c r="F3" s="16"/>
       <c r="G3" s="17"/>
       <c r="H3" s="17"/>
       <c r="I3" s="17"/>
       <c r="J3" s="18"/>
     </row>
     <row r="4" ht="49.5" customHeight="1">
-      <c r="A4" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" s="13" t="s">
-        <v>12</v>
-      </c>
+      <c r="A4" s="19"/>
+      <c r="B4" s="20"/>
       <c r="C4" s="14">
         <v>2.0</v>
       </c>
-      <c r="D4" s="20" t="s">
+      <c r="D4" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" s="16"/>
       <c r="G4" s="17"/>
       <c r="H4" s="17"/>
       <c r="I4" s="17"/>
       <c r="J4" s="18"/>
     </row>
     <row r="5" ht="49.5" customHeight="1">
-      <c r="A5" s="21" t="s">
-        <v>18</v>
+      <c r="A5" s="22" t="s">
+        <v>17</v>
       </c>
       <c r="B5" s="13" t="s">
         <v>12</v>
@@ -738,11 +750,11 @@
       <c r="C5" s="14">
         <v>3.0</v>
       </c>
-      <c r="D5" s="22" t="s">
-        <v>19</v>
+      <c r="D5" s="21" t="s">
+        <v>18</v>
       </c>
       <c r="E5" s="16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F5" s="23"/>
       <c r="G5" s="24"/>
@@ -751,110 +763,124 @@
       <c r="J5" s="18"/>
     </row>
     <row r="6" ht="49.5" customHeight="1">
-      <c r="A6" s="25"/>
-      <c r="B6" s="26" t="s">
-        <v>21</v>
-      </c>
+      <c r="A6" s="20"/>
+      <c r="B6" s="20"/>
       <c r="C6" s="14">
         <v>4.0</v>
       </c>
-      <c r="D6" s="22" t="s">
-        <v>22</v>
+      <c r="D6" s="25" t="s">
+        <v>20</v>
       </c>
-      <c r="E6" s="16"/>
+      <c r="E6" s="16" t="s">
+        <v>21</v>
+      </c>
       <c r="F6" s="23"/>
       <c r="G6" s="24"/>
       <c r="H6" s="17"/>
-      <c r="I6" s="24" t="s">
-        <v>23</v>
-      </c>
+      <c r="I6" s="24"/>
       <c r="J6" s="18"/>
     </row>
     <row r="7" ht="49.5" customHeight="1">
-      <c r="A7" s="27"/>
-      <c r="B7" s="25"/>
+      <c r="A7" s="19"/>
+      <c r="B7" s="20"/>
       <c r="C7" s="14">
         <v>5.0</v>
       </c>
-      <c r="D7" s="22" t="s">
-        <v>24</v>
+      <c r="D7" s="25" t="s">
+        <v>22</v>
       </c>
-      <c r="E7" s="16" t="s">
-        <v>25</v>
+      <c r="E7" s="16"/>
+      <c r="F7" s="16" t="s">
+        <v>23</v>
       </c>
-      <c r="F7" s="23"/>
       <c r="G7" s="24"/>
       <c r="H7" s="17"/>
       <c r="I7" s="24"/>
       <c r="J7" s="18"/>
     </row>
     <row r="8" ht="49.5" customHeight="1">
-      <c r="A8" s="28" t="s">
-        <v>26</v>
+      <c r="A8" s="26" t="s">
+        <v>24</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="C8" s="14">
         <v>6.0</v>
       </c>
-      <c r="D8" s="22" t="s">
-        <v>27</v>
+      <c r="D8" s="25" t="s">
+        <v>26</v>
       </c>
-      <c r="E8" s="16" t="s">
-        <v>28</v>
-      </c>
+      <c r="E8" s="16"/>
       <c r="F8" s="16"/>
       <c r="G8" s="24"/>
       <c r="H8" s="17"/>
-      <c r="I8" s="17"/>
+      <c r="I8" s="24" t="s">
+        <v>27</v>
+      </c>
       <c r="J8" s="18"/>
     </row>
     <row r="9" ht="49.5" customHeight="1">
-      <c r="A9" s="29" t="s">
-        <v>29</v>
-      </c>
-      <c r="B9" s="30" t="s">
-        <v>12</v>
-      </c>
+      <c r="A9" s="19"/>
+      <c r="B9" s="19"/>
       <c r="C9" s="14">
         <v>7.0</v>
       </c>
-      <c r="D9" s="22" t="s">
-        <v>30</v>
+      <c r="D9" s="25" t="s">
+        <v>28</v>
       </c>
-      <c r="E9" s="16"/>
-      <c r="F9" s="23"/>
-      <c r="G9" s="24" t="s">
-        <v>31</v>
+      <c r="E9" s="16" t="s">
+        <v>29</v>
       </c>
+      <c r="F9" s="16"/>
+      <c r="G9" s="24"/>
       <c r="H9" s="17"/>
       <c r="I9" s="17"/>
       <c r="J9" s="18"/>
     </row>
-    <row r="10" ht="40.5" customHeight="1">
-      <c r="A10" s="31"/>
-      <c r="B10" s="31"/>
-      <c r="C10" s="31"/>
-      <c r="D10" s="31"/>
-      <c r="E10" s="31"/>
-      <c r="F10" s="31"/>
-      <c r="G10" s="31"/>
-      <c r="H10" s="31"/>
-      <c r="I10" s="31"/>
-      <c r="J10" s="31"/>
+    <row r="10" ht="45.0" customHeight="1">
+      <c r="A10" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="14">
+        <v>8.0</v>
+      </c>
+      <c r="D10" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10" s="16"/>
+      <c r="F10" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="G10" s="24"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="17"/>
+      <c r="J10" s="18"/>
     </row>
     <row r="11" ht="40.5" customHeight="1">
-      <c r="A11" s="31"/>
-      <c r="B11" s="31"/>
-      <c r="C11" s="31"/>
-      <c r="D11" s="31"/>
-      <c r="E11" s="31"/>
-      <c r="F11" s="31"/>
-      <c r="G11" s="31"/>
-      <c r="H11" s="31"/>
-      <c r="I11" s="31"/>
-      <c r="J11" s="31"/>
+      <c r="A11" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="14">
+        <v>9.0</v>
+      </c>
+      <c r="D11" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="E11" s="16"/>
+      <c r="F11" s="23"/>
+      <c r="G11" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="H11" s="17"/>
+      <c r="I11" s="17"/>
+      <c r="J11" s="18"/>
     </row>
     <row r="12" ht="40.5" customHeight="1">
       <c r="A12" s="31"/>
@@ -12653,13 +12679,17 @@
       <c r="J994" s="31"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="10">
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="G1:I1"/>
     <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="B5:B7"/>
     <mergeCell ref="A5:A7"/>
-    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:B9"/>
   </mergeCells>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>

</xml_diff>